<commit_message>
Vault backup: 20/05/24 19:34:35 ASUS
Affected files:
Motorrad.xlsx
</commit_message>
<xml_diff>
--- a/Motorrad.xlsx
+++ b/Motorrad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\2023_24_4BHITS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD559215-89F2-44B7-BE68-3E651B3C2023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF4D96F-C804-40C4-A701-72D75AEB04FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{025C3977-F6EF-40A4-9376-783BE05C9CA1}"/>
+    <workbookView xWindow="420" yWindow="2055" windowWidth="21600" windowHeight="11295" xr2:uid="{025C3977-F6EF-40A4-9376-783BE05C9CA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Händler</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Artikel</t>
   </si>
   <si>
-    <t>Ölfilter</t>
-  </si>
-  <si>
     <t>Bremse v</t>
   </si>
   <si>
@@ -66,12 +63,6 @@
   </si>
   <si>
     <t>Amazon</t>
-  </si>
-  <si>
-    <t>Louis</t>
-  </si>
-  <si>
-    <t>https://www.louis.at/de/k-n-kartuschen-oelfilter-fuer-diverse-fahrzeuge-10051020?filter_bike_id=3546&amp;filter_article_number=10051032</t>
   </si>
   <si>
     <t>Radical</t>
@@ -149,10 +140,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -179,17 +169,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82BF334F-8F49-43F5-A119-DDF0E6C5468C}" name="Tabelle1" displayName="Tabelle1" ref="A1:E9" totalsRowCount="1">
-  <autoFilter ref="A1:E8" xr:uid="{82BF334F-8F49-43F5-A119-DDF0E6C5468C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E7">
-    <sortCondition ref="D1:D7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82BF334F-8F49-43F5-A119-DDF0E6C5468C}" name="Tabelle1" displayName="Tabelle1" ref="A1:E8" totalsRowCount="1">
+  <autoFilter ref="A1:E7" xr:uid="{82BF334F-8F49-43F5-A119-DDF0E6C5468C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E6">
+    <sortCondition ref="D1:D6"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{3CDF4D52-7C64-4592-8565-14F8F1F27490}" name="Artikel"/>
     <tableColumn id="2" xr3:uid="{504ADE62-2556-44C1-B06C-2E799C9E4421}" name="Händler"/>
     <tableColumn id="5" xr3:uid="{1A4C1715-BB69-446D-97CF-68D787C5A759}" name="Gekauft?"/>
     <tableColumn id="3" xr3:uid="{0D55CAA1-49CC-492A-8BC8-826FF45CE21E}" name="Preis" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
-      <totalsRowFormula>SUM(D2:D8)</totalsRowFormula>
+      <totalsRowFormula>SUM(D2:D7)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{E32DEDDB-5A32-4187-881D-E684A6826652}" name="Link"/>
   </tableColumns>
@@ -514,20 +504,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D18C22E2-FEFB-4B56-9AA5-E0909CAFCB9F}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="130.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="130.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -535,135 +525,121 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>14.99</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>14.99</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>1.79</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>2.99</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2">
-        <v>14.99</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="2">
-        <v>14.99</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.79</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="2">
-        <v>2.99</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>45.13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2">
-        <v>45.13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2">
-        <v>8.99</v>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>11.79</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="2">
-        <v>11.79</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D9" s="2">
-        <f>SUM(D2:D8)</f>
-        <v>100.66999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E12" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f>SUM(D2:D7)</f>
+        <v>91.68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>